<commit_message>
commit on 14th sep
</commit_message>
<xml_diff>
--- a/proVidioETG/testDate/GiftCertificateCodesForGc.xlsx
+++ b/proVidioETG/testDate/GiftCertificateCodesForGc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t xml:space="preserve">codes for  only Gc</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">RDYHRJYOZFRIKDDT </t>
   </si>
   <si>
+    <t xml:space="preserve">PYGVMDQPPHKYLLYD </t>
+  </si>
+  <si>
     <t xml:space="preserve">TSYTLQMVLSJJYHRP </t>
   </si>
   <si>
@@ -41,6 +44,18 @@
   </si>
   <si>
     <t xml:space="preserve">SPQKTWFWSTPIOQOO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZLQYYISHRYODIRQG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WTCIQJTMWWJSCSFH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VYKZILJIYJSYKHPR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JJTYTAFLPKCRHRYO </t>
   </si>
 </sst>
 </file>
@@ -147,11 +162,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -232,10 +247,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -250,7 +265,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -260,49 +275,59 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
+      <c r="A5" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
+      <c r="A6" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2"/>
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
@@ -312,6 +337,9 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>